<commit_message>
Versão que está instalada no cliente
</commit_message>
<xml_diff>
--- a/Versões Customizadas/LJB-105K (curva acentuada para atingir -105°C quando na verdade é 68°C.xlsx
+++ b/Versões Customizadas/LJB-105K (curva acentuada para atingir -105°C quando na verdade é 68°C.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Indka(R)\JJCientifica\Liofilizador\Firmware\FD_Slave_Board\Versões Customizadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B34451DA-500D-4BC5-B1B0-F9EEC1701FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E25307F-BAE5-41DD-8012-DA9522D60C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C464691A-4E6C-4B15-9F3D-E838553165C9}"/>
   </bookViews>
@@ -144,10 +144,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$B$1:$B$94</c:f>
+              <c:f>Planilha1!$B$1:$B$111</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="94"/>
+                <c:ptCount val="111"/>
                 <c:pt idx="0">
                   <c:v>25</c:v>
                 </c:pt>
@@ -362,73 +362,124 @@
                   <c:v>-45</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>-46.07</c:v>
+                  <c:v>-46.012999999999998</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>-47.28</c:v>
+                  <c:v>-47.052</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>-48.63</c:v>
+                  <c:v>-48.116999999999997</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>-50.12</c:v>
+                  <c:v>-49.207999999999998</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>-51.75</c:v>
+                  <c:v>-50.325000000000003</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>-53.52</c:v>
+                  <c:v>-51.468000000000004</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>-55.43</c:v>
+                  <c:v>-52.637</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>-57.480000000000004</c:v>
+                  <c:v>-53.832000000000001</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>-59.67</c:v>
+                  <c:v>-55.052999999999997</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>-62</c:v>
+                  <c:v>-56.3</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>-64.47</c:v>
+                  <c:v>-57.573</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>-67.08</c:v>
+                  <c:v>-58.872</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>-69.83</c:v>
+                  <c:v>-60.197000000000003</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>-72.72</c:v>
+                  <c:v>-61.548000000000002</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>-75.75</c:v>
+                  <c:v>-62.924999999999997</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>-78.92</c:v>
+                  <c:v>-64.328000000000003</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>-82.23</c:v>
+                  <c:v>-65.757000000000005</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>-85.68</c:v>
+                  <c:v>-67.212000000000003</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>-89.27000000000001</c:v>
+                  <c:v>-68.692999999999998</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>-93</c:v>
+                  <c:v>-70.2</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>-96.87</c:v>
+                  <c:v>-71.733000000000004</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>-100.88</c:v>
+                  <c:v>-73.292000000000002</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>-105.03</c:v>
+                  <c:v>-74.876999999999995</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>-76.488</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-78.125</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>-79.787999999999997</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>-81.477000000000004</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-83.192000000000007</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>-84.932999999999993</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>-86.7</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>-88.492999999999995</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>-90.311999999999998</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>-92.156999999999996</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>-94.027999999999992</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>-95.924999999999997</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>-97.847999999999999</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>-99.796999999999997</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>-101.77199999999999</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>-103.773</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>-105.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -436,7 +487,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D43D-4502-8A14-CF4CE5CC8C57}"/>
+              <c16:uniqueId val="{00000000-5EB5-4299-978E-D187CF09BD79}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -449,11 +500,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1699410447"/>
-        <c:axId val="1699407119"/>
+        <c:axId val="1333050287"/>
+        <c:axId val="1333045711"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1699410447"/>
+        <c:axId val="1333050287"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -495,7 +546,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1699407119"/>
+        <c:crossAx val="1333045711"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -503,7 +554,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1699407119"/>
+        <c:axId val="1333045711"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -554,7 +605,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1699410447"/>
+        <c:crossAx val="1333050287"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1170,23 +1221,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>528637</xdr:colOff>
-      <xdr:row>92</xdr:row>
-      <xdr:rowOff>6</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>166687</xdr:colOff>
-      <xdr:row>106</xdr:row>
-      <xdr:rowOff>76206</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1">
+        <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC61E85C-531D-4591-92DC-161E022F890C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BB0BD19-B877-4C15-99DB-59552C6C68EF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1506,8 +1557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1024B6AE-A9AB-40AC-A2E0-919922791783}">
   <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2085,7 +2136,7 @@
         <v>-45</v>
       </c>
       <c r="D71">
-        <v>7.0000000000000007E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2093,8 +2144,8 @@
         <v>-46</v>
       </c>
       <c r="B72" s="1">
-        <f t="shared" ref="B72:B94" si="0">A72-(((A72+45)*(A72+45))*$D$71)</f>
-        <v>-46.07</v>
+        <f>A72-(((A72+45)*(A72+45))*$D$71)</f>
+        <v>-46.012999999999998</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2102,12 +2153,12 @@
         <v>-47</v>
       </c>
       <c r="B73" s="1">
-        <f t="shared" si="0"/>
-        <v>-47.28</v>
+        <f>A73-(((A73+45)*(A73+45))*$D$71)</f>
+        <v>-47.052</v>
       </c>
       <c r="D73">
-        <f>B94</f>
-        <v>-105.03</v>
+        <f>B110</f>
+        <v>-103.773</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2115,8 +2166,8 @@
         <v>-48</v>
       </c>
       <c r="B74" s="1">
-        <f t="shared" si="0"/>
-        <v>-48.63</v>
+        <f t="shared" ref="B72:B118" si="0">A74-(((A74+45)*(A74+45))*$D$71)</f>
+        <v>-48.116999999999997</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2125,7 +2176,7 @@
       </c>
       <c r="B75" s="1">
         <f t="shared" si="0"/>
-        <v>-50.12</v>
+        <v>-49.207999999999998</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2134,7 +2185,7 @@
       </c>
       <c r="B76" s="1">
         <f t="shared" si="0"/>
-        <v>-51.75</v>
+        <v>-50.325000000000003</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2143,7 +2194,7 @@
       </c>
       <c r="B77" s="1">
         <f t="shared" si="0"/>
-        <v>-53.52</v>
+        <v>-51.468000000000004</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2152,7 +2203,7 @@
       </c>
       <c r="B78" s="1">
         <f t="shared" si="0"/>
-        <v>-55.43</v>
+        <v>-52.637</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2161,7 +2212,7 @@
       </c>
       <c r="B79" s="1">
         <f t="shared" si="0"/>
-        <v>-57.480000000000004</v>
+        <v>-53.832000000000001</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2170,7 +2221,7 @@
       </c>
       <c r="B80" s="1">
         <f t="shared" si="0"/>
-        <v>-59.67</v>
+        <v>-55.052999999999997</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -2179,7 +2230,7 @@
       </c>
       <c r="B81" s="1">
         <f t="shared" si="0"/>
-        <v>-62</v>
+        <v>-56.3</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -2188,7 +2239,7 @@
       </c>
       <c r="B82" s="1">
         <f t="shared" si="0"/>
-        <v>-64.47</v>
+        <v>-57.573</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -2197,7 +2248,7 @@
       </c>
       <c r="B83" s="1">
         <f t="shared" si="0"/>
-        <v>-67.08</v>
+        <v>-58.872</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -2206,7 +2257,7 @@
       </c>
       <c r="B84" s="1">
         <f t="shared" si="0"/>
-        <v>-69.83</v>
+        <v>-60.197000000000003</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -2215,7 +2266,7 @@
       </c>
       <c r="B85" s="1">
         <f t="shared" si="0"/>
-        <v>-72.72</v>
+        <v>-61.548000000000002</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -2224,7 +2275,7 @@
       </c>
       <c r="B86" s="1">
         <f t="shared" si="0"/>
-        <v>-75.75</v>
+        <v>-62.924999999999997</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -2233,7 +2284,7 @@
       </c>
       <c r="B87" s="1">
         <f t="shared" si="0"/>
-        <v>-78.92</v>
+        <v>-64.328000000000003</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -2242,7 +2293,7 @@
       </c>
       <c r="B88" s="1">
         <f t="shared" si="0"/>
-        <v>-82.23</v>
+        <v>-65.757000000000005</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -2251,7 +2302,7 @@
       </c>
       <c r="B89" s="1">
         <f t="shared" si="0"/>
-        <v>-85.68</v>
+        <v>-67.212000000000003</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -2260,7 +2311,7 @@
       </c>
       <c r="B90" s="1">
         <f t="shared" si="0"/>
-        <v>-89.27000000000001</v>
+        <v>-68.692999999999998</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -2269,7 +2320,7 @@
       </c>
       <c r="B91" s="1">
         <f t="shared" si="0"/>
-        <v>-93</v>
+        <v>-70.2</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -2278,7 +2329,7 @@
       </c>
       <c r="B92" s="1">
         <f t="shared" si="0"/>
-        <v>-96.87</v>
+        <v>-71.733000000000004</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -2287,7 +2338,7 @@
       </c>
       <c r="B93" s="1">
         <f t="shared" si="0"/>
-        <v>-100.88</v>
+        <v>-73.292000000000002</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -2296,175 +2347,271 @@
       </c>
       <c r="B94" s="1">
         <f t="shared" si="0"/>
-        <v>-105.03</v>
+        <v>-74.876999999999995</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>-69</v>
       </c>
+      <c r="B95" s="1">
+        <f t="shared" si="0"/>
+        <v>-76.488</v>
+      </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>-70</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B96" s="1">
+        <f t="shared" si="0"/>
+        <v>-78.125</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>-71</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B97" s="1">
+        <f t="shared" si="0"/>
+        <v>-79.787999999999997</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>-72</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B98" s="1">
+        <f t="shared" si="0"/>
+        <v>-81.477000000000004</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>-73</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B99" s="1">
+        <f t="shared" si="0"/>
+        <v>-83.192000000000007</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>-74</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B100" s="1">
+        <f t="shared" si="0"/>
+        <v>-84.932999999999993</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>-75</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B101" s="1">
+        <f t="shared" si="0"/>
+        <v>-86.7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>-76</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B102" s="1">
+        <f t="shared" si="0"/>
+        <v>-88.492999999999995</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>-77</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B103" s="1">
+        <f t="shared" si="0"/>
+        <v>-90.311999999999998</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>-78</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B104" s="1">
+        <f t="shared" si="0"/>
+        <v>-92.156999999999996</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>-79</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B105" s="1">
+        <f t="shared" si="0"/>
+        <v>-94.027999999999992</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>-80</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B106" s="1">
+        <f t="shared" si="0"/>
+        <v>-95.924999999999997</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>-81</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B107" s="1">
+        <f t="shared" si="0"/>
+        <v>-97.847999999999999</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>-82</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B108" s="1">
+        <f t="shared" si="0"/>
+        <v>-99.796999999999997</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>-83</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B109" s="1">
+        <f t="shared" si="0"/>
+        <v>-101.77199999999999</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>-84</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B110" s="1">
+        <f t="shared" si="0"/>
+        <v>-103.773</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>-85</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B111" s="1">
+        <f t="shared" si="0"/>
+        <v>-105.8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>-86</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B112" s="1">
+        <f t="shared" si="0"/>
+        <v>-107.85299999999999</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>-87</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B113" s="1">
+        <f t="shared" si="0"/>
+        <v>-109.932</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>-88</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B114" s="1">
+        <f t="shared" si="0"/>
+        <v>-112.03700000000001</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>-89</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B115" s="1">
+        <f t="shared" si="0"/>
+        <v>-114.16800000000001</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>-90</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B116" s="1">
+        <f t="shared" si="0"/>
+        <v>-116.325</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>-91</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B117" s="1">
+        <f t="shared" si="0"/>
+        <v>-118.508</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>-92</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B118" s="1">
+        <f t="shared" si="0"/>
+        <v>-120.717</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>-93</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>-94</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>-95</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>-96</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>-97</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>-98</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>-99</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>-100</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>-101</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>-102</v>
       </c>

</xml_diff>

<commit_message>
commitado para postar no github
</commit_message>
<xml_diff>
--- a/Versões Customizadas/LJB-105K (curva acentuada para atingir -105°C quando na verdade é 68°C.xlsx
+++ b/Versões Customizadas/LJB-105K (curva acentuada para atingir -105°C quando na verdade é 68°C.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Indka(R)\JJCientifica\Liofilizador\Firmware\FD_Slave_Board\Versões Customizadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E25307F-BAE5-41DD-8012-DA9522D60C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725BBADD-ACBE-49F6-AB0D-4CDE141EE3F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C464691A-4E6C-4B15-9F3D-E838553165C9}"/>
   </bookViews>
@@ -1557,8 +1557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1024B6AE-A9AB-40AC-A2E0-919922791783}">
   <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B111"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="B118" sqref="B118:B131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2166,7 +2166,7 @@
         <v>-48</v>
       </c>
       <c r="B74" s="1">
-        <f t="shared" ref="B72:B118" si="0">A74-(((A74+45)*(A74+45))*$D$71)</f>
+        <f t="shared" ref="B74:B131" si="0">A74-(((A74+45)*(A74+45))*$D$71)</f>
         <v>-48.116999999999997</v>
       </c>
     </row>
@@ -2570,65 +2570,117 @@
       <c r="A119" s="1">
         <v>-93</v>
       </c>
+      <c r="B119" s="1">
+        <f t="shared" si="0"/>
+        <v>-122.952</v>
+      </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>-94</v>
       </c>
+      <c r="B120" s="1">
+        <f t="shared" si="0"/>
+        <v>-125.21299999999999</v>
+      </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>-95</v>
       </c>
+      <c r="B121" s="1">
+        <f t="shared" si="0"/>
+        <v>-127.5</v>
+      </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>-96</v>
       </c>
+      <c r="B122" s="1">
+        <f t="shared" si="0"/>
+        <v>-129.81299999999999</v>
+      </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>-97</v>
       </c>
+      <c r="B123" s="1">
+        <f t="shared" si="0"/>
+        <v>-132.15199999999999</v>
+      </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>-98</v>
       </c>
+      <c r="B124" s="1">
+        <f t="shared" si="0"/>
+        <v>-134.517</v>
+      </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>-99</v>
       </c>
+      <c r="B125" s="1">
+        <f t="shared" si="0"/>
+        <v>-136.90800000000002</v>
+      </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>-100</v>
       </c>
+      <c r="B126" s="1">
+        <f t="shared" si="0"/>
+        <v>-139.32499999999999</v>
+      </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>-101</v>
       </c>
+      <c r="B127" s="1">
+        <f t="shared" si="0"/>
+        <v>-141.768</v>
+      </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>-102</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B128" s="1">
+        <f t="shared" si="0"/>
+        <v>-144.23699999999999</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>-103</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B129" s="1">
+        <f t="shared" si="0"/>
+        <v>-146.732</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>-104</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B130" s="1">
+        <f t="shared" si="0"/>
+        <v>-149.25299999999999</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>-105</v>
+      </c>
+      <c r="B131" s="1">
+        <f t="shared" si="0"/>
+        <v>-151.80000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>